<commit_message>
initial commit of new br
</commit_message>
<xml_diff>
--- a/Used_MembersID.xlsx
+++ b/Used_MembersID.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,8 +441,15 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>56122</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>56122</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>79086</v>
       </c>
     </row>
   </sheetData>

</xml_diff>